<commit_message>
some progress on FSM
</commit_message>
<xml_diff>
--- a/Music.xlsx
+++ b/Music.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Hz</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>b2</t>
+  </si>
+  <si>
+    <t>note</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:D25"/>
+  <dimension ref="A4:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
@@ -424,7 +427,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -437,8 +440,11 @@
       <c r="D4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -452,8 +458,12 @@
         <f>200000/C5</f>
         <v>3058.103975535168</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <f>D5/2</f>
+        <v>1529.051987767584</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -467,8 +477,12 @@
         <f t="shared" ref="D6:D25" si="0">200000/C6</f>
         <v>2724.7956403269754</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <f t="shared" ref="E6:E25" si="1">D6/2</f>
+        <v>1362.3978201634877</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -482,8 +496,12 @@
         <f t="shared" si="0"/>
         <v>2427.1844660194174</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>1213.5922330097087</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -497,8 +515,12 @@
         <f t="shared" si="0"/>
         <v>2290.950744558992</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>1145.475372279496</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -512,8 +534,12 @@
         <f t="shared" si="0"/>
         <v>2041.0245943463619</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>1020.512297173181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -527,8 +553,12 @@
         <f t="shared" si="0"/>
         <v>1818.1818181818182</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>909.09090909090912</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -542,8 +572,12 @@
         <f t="shared" si="0"/>
         <v>1619.8266785453957</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>809.91333927269784</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -557,8 +591,12 @@
         <f t="shared" si="0"/>
         <v>1529.051987767584</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>764.52599388379201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -572,8 +610,12 @@
         <f t="shared" si="0"/>
         <v>1362.3978201634877</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>681.19891008174386</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -587,8 +629,12 @@
         <f t="shared" si="0"/>
         <v>1213.4891453395951</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>606.74457266979755</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -602,8 +648,12 @@
         <f t="shared" si="0"/>
         <v>1145.3835316755815</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>572.69176583779074</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -617,8 +667,12 @@
         <f t="shared" si="0"/>
         <v>1020.4185756997521</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>510.20928784987603</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -632,8 +686,12 @@
         <f t="shared" si="0"/>
         <v>909.09090909090912</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>454.54545454545456</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -647,8 +705,12 @@
         <f t="shared" si="0"/>
         <v>809.90677972965307</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>404.95338986482653</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -662,8 +724,12 @@
         <f t="shared" si="0"/>
         <v>764.45001643567537</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>382.22500821783768</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -677,8 +743,12 @@
         <f t="shared" si="0"/>
         <v>681.04813307680513</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>340.52406653840256</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -692,8 +762,12 @@
         <f t="shared" si="0"/>
         <v>606.74457266979755</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>303.37228633489877</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -707,8 +781,12 @@
         <f t="shared" si="0"/>
         <v>572.69176583779074</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>286.34588291889537</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -722,8 +800,12 @@
         <f t="shared" si="0"/>
         <v>510.21058942078344</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>255.10529471039172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -737,8 +819,12 @@
         <f t="shared" si="0"/>
         <v>454.54545454545456</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>227.27272727272728</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -751,6 +837,10 @@
       <c r="D25">
         <f t="shared" si="0"/>
         <v>404.95420980272655</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>202.47710490136328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>